<commit_message>
Need to adjust files
</commit_message>
<xml_diff>
--- a/ScansSep24.xlsx
+++ b/ScansSep24.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diego\git\6s7p\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961DFFD2-F0C8-40EF-9B14-DAFD53AFCD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3221CEF-9A9C-4C7F-9302-ADF53F604D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D080EF3-E891-48AE-ADEA-FE9E1802C9D2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3D080EF3-E891-48AE-ADEA-FE9E1802C9D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>